<commit_message>
work on data for preselection
</commit_message>
<xml_diff>
--- a/Data prep/macro_data.xlsx
+++ b/Data prep/macro_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lena/Git/GDP-nowcasting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lena/Git/GDP-nowcasting/Data prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339EAC8B-DB90-3245-8FBC-A30BDB1DAE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E052FB-7934-A94E-9221-12401AB270E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1480" windowWidth="27240" windowHeight="15500" xr2:uid="{31849CCF-4493-4A40-A62C-CB2ED16BC9FE}"/>
+    <workbookView xWindow="1080" yWindow="580" windowWidth="27240" windowHeight="15500" activeTab="2" xr2:uid="{31849CCF-4493-4A40-A62C-CB2ED16BC9FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="IP index" sheetId="3" r:id="rId3"/>
     <sheet name="DE ESI" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -449,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97B4AF1-7542-E049-9574-4D535DF60CA2}">
   <dimension ref="A3:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -495,7 +495,7 @@
   <dimension ref="A1:B130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1546,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FDF1A05-402E-CF41-9944-E6812286EFC4}">
   <dimension ref="A1:C388"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1579,8 +1579,8 @@
         <v>78</v>
       </c>
       <c r="C3">
-        <f>(B2-B3)/B2*100</f>
-        <v>1.1406844106463949</v>
+        <f xml:space="preserve"> (B3-B2)/B2*100</f>
+        <v>-1.1406844106463949</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1591,8 +1591,8 @@
         <v>77.3</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C67" si="0">(B3-B4)/B3*100</f>
-        <v>0.89743589743590102</v>
+        <f t="shared" ref="C4:C67" si="0" xml:space="preserve"> (B4-B3)/B3*100</f>
+        <v>-0.89743589743590102</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0.90556274256145264</v>
+        <v>-0.90556274256145264</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0.913838120104424</v>
+        <v>-0.913838120104424</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>-3.5573122529644117</v>
+        <v>3.5573122529644117</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1640,7 +1640,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>3.0534351145038063</v>
+        <v>-3.0534351145038063</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1652,7 +1652,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>1.0498687664041957</v>
+        <v>-1.0498687664041957</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0.39787798408489566</v>
+        <v>-0.39787798408489566</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>-1.4647137150466161</v>
+        <v>1.4647137150466161</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>-1.1811023622047132</v>
+        <v>1.1811023622047132</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1700,7 +1700,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>0.12970168612191224</v>
+        <v>-0.12970168612191224</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>-1.5584415584415621</v>
+        <v>1.5584415584415621</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1724,7 +1724,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>-1.0230179028132955</v>
+        <v>1.0230179028132955</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>2.405063291139248</v>
+        <v>-2.405063291139248</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.12970168612191224</v>
+        <v>-0.12970168612191224</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1760,7 +1760,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>1.0389610389610353</v>
+        <v>-1.0389610389610353</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>1.1811023622047319</v>
+        <v>-1.1811023622047319</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>1.9920318725099602</v>
+        <v>-1.9920318725099602</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>-0.94850948509485489</v>
+        <v>0.94850948509485489</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1808,7 +1808,7 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>1.0738255033557009</v>
+        <v>-1.0738255033557009</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1820,7 +1820,7 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>0.13568521031208755</v>
+        <v>-0.13568521031208755</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1832,7 +1832,7 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>1.4945652173912967</v>
+        <v>-1.4945652173912967</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1844,7 +1844,7 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>1.9310344827586285</v>
+        <v>-1.9310344827586285</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>0.14064697609000609</v>
+        <v>-0.14064697609000609</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>1.5492957746478793</v>
+        <v>-1.5492957746478793</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1880,7 +1880,7 @@
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>0.14306151645208659</v>
+        <v>-0.14306151645208659</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1892,7 +1892,7 @@
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>0.85959885386818669</v>
+        <v>-0.85959885386818669</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1904,7 +1904,7 @@
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>0.28901734104046656</v>
+        <v>-0.28901734104046656</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>0.434782608695648</v>
+        <v>-0.434782608695648</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1928,7 +1928,7 @@
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>2.0378457059679849</v>
+        <v>-2.0378457059679849</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1940,7 +1940,7 @@
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>-4.1604754829123287</v>
+        <v>4.1604754829123287</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1952,7 +1952,7 @@
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>0.42796005706133694</v>
+        <v>-0.42796005706133694</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>0.42979942693409334</v>
+        <v>-0.42979942693409334</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>-0.86330935251797747</v>
+        <v>0.86330935251797747</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>0.71326676176890158</v>
+        <v>-0.71326676176890158</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>-1.7241379310344869</v>
+        <v>1.7241379310344869</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2024,7 +2024,7 @@
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>0.70621468926553677</v>
+        <v>-0.70621468926553677</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>-1.4224751066856329</v>
+        <v>1.4224751066856329</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2048,7 +2048,7 @@
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>0.42075736325385293</v>
+        <v>-0.42075736325385293</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>-0.28169014084507443</v>
+        <v>0.28169014084507443</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>0.28089887640449834</v>
+        <v>-0.28089887640449834</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>-1.4084507042253522</v>
+        <v>1.4084507042253522</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2108,7 +2108,7 @@
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>-1.9444444444444524</v>
+        <v>1.9444444444444524</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -2120,7 +2120,7 @@
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
-        <v>0.2724795640327014</v>
+        <v>-0.2724795640327014</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>-0.27322404371585085</v>
+        <v>0.27322404371585085</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>1.9073569482288906</v>
+        <v>-1.9073569482288906</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2156,7 +2156,7 @@
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>-1.3888888888888888</v>
+        <v>1.3888888888888888</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>0.68493150684931503</v>
+        <v>-0.68493150684931503</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>-0.55172413793104236</v>
+        <v>0.55172413793104236</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2192,7 +2192,7 @@
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
-        <v>-0.54869684499312954</v>
+        <v>0.54869684499312954</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2204,7 +2204,7 @@
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>0.95497953615280073</v>
+        <v>-0.95497953615280073</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
-        <v>0.41322314049586389</v>
+        <v>-0.41322314049586389</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="C57">
         <f t="shared" si="0"/>
-        <v>0.9681881051175697</v>
+        <v>-0.9681881051175697</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2240,7 +2240,7 @@
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
-        <v>-1.8156424581005748</v>
+        <v>1.8156424581005748</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2252,7 +2252,7 @@
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
-        <v>2.6063100137174287</v>
+        <v>-2.6063100137174287</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2264,7 +2264,7 @@
       </c>
       <c r="C60">
         <f t="shared" si="0"/>
-        <v>-0.84507042253520326</v>
+        <v>0.84507042253520326</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
-        <v>-0.41899441340783716</v>
+        <v>0.41899441340783716</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -2288,7 +2288,7 @@
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
-        <v>0.13908205841447638</v>
+        <v>-0.13908205841447638</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="C64">
         <f t="shared" si="0"/>
-        <v>-0.27855153203343019</v>
+        <v>0.27855153203343019</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="C65">
         <f t="shared" si="0"/>
-        <v>0.69444444444444442</v>
+        <v>-0.69444444444444442</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="C66">
         <f t="shared" si="0"/>
-        <v>-1.2587412587412667</v>
+        <v>1.2587412587412667</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2348,7 +2348,7 @@
       </c>
       <c r="C67">
         <f t="shared" si="0"/>
-        <v>0.13812154696133774</v>
+        <v>-0.13812154696133774</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2359,8 +2359,8 @@
         <v>71.599999999999994</v>
       </c>
       <c r="C68">
-        <f t="shared" ref="C68:C131" si="1">(B67-B68)/B67*100</f>
-        <v>0.9681881051175697</v>
+        <f t="shared" ref="C68:C131" si="1" xml:space="preserve"> (B68-B67)/B67*100</f>
+        <v>-0.9681881051175697</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -2372,7 +2372,7 @@
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
-        <v>-1.8156424581005748</v>
+        <v>1.8156424581005748</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
-        <v>-0.41152263374485198</v>
+        <v>0.41152263374485198</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="C71">
         <f t="shared" si="1"/>
-        <v>1.2295081967213193</v>
+        <v>-1.2295081967213193</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -2408,7 +2408,7 @@
       </c>
       <c r="C72">
         <f t="shared" si="1"/>
-        <v>-1.2448132780083065</v>
+        <v>1.2448132780083065</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2420,7 +2420,7 @@
       </c>
       <c r="C73">
         <f t="shared" si="1"/>
-        <v>-0.13661202185791574</v>
+        <v>0.13661202185791574</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2432,7 +2432,7 @@
       </c>
       <c r="C74">
         <f t="shared" si="1"/>
-        <v>0.68212824010914053</v>
+        <v>-0.68212824010914053</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2444,7 +2444,7 @@
       </c>
       <c r="C75">
         <f t="shared" si="1"/>
-        <v>-0.54945054945055727</v>
+        <v>0.54945054945055727</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2456,7 +2456,7 @@
       </c>
       <c r="C76">
         <f t="shared" si="1"/>
-        <v>-1.0928961748633841</v>
+        <v>1.0928961748633841</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2468,7 +2468,7 @@
       </c>
       <c r="C77">
         <f t="shared" si="1"/>
-        <v>0.40540540540540154</v>
+        <v>-0.40540540540540154</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -2480,7 +2480,7 @@
       </c>
       <c r="C78">
         <f t="shared" si="1"/>
-        <v>0.67842605156037983</v>
+        <v>-0.67842605156037983</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -2492,7 +2492,7 @@
       </c>
       <c r="C79">
         <f t="shared" si="1"/>
-        <v>-2.7322404371584699</v>
+        <v>2.7322404371584699</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2504,7 +2504,7 @@
       </c>
       <c r="C80">
         <f t="shared" si="1"/>
-        <v>-1.0638297872340388</v>
+        <v>1.0638297872340388</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2516,7 +2516,7 @@
       </c>
       <c r="C81">
         <f t="shared" si="1"/>
-        <v>2.8947368421052668</v>
+        <v>-2.8947368421052668</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -2528,7 +2528,7 @@
       </c>
       <c r="C82">
         <f t="shared" si="1"/>
-        <v>-0.81300813008131234</v>
+        <v>0.81300813008131234</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="C83">
         <f t="shared" si="1"/>
-        <v>-1.4784946236559062</v>
+        <v>1.4784946236559062</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2552,7 +2552,7 @@
       </c>
       <c r="C84">
         <f t="shared" si="1"/>
-        <v>-0.3973509933774797</v>
+        <v>0.3973509933774797</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="C85">
         <f t="shared" si="1"/>
-        <v>-0.92348284960422544</v>
+        <v>0.92348284960422544</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2576,7 +2576,7 @@
       </c>
       <c r="C86">
         <f t="shared" si="1"/>
-        <v>-0.78431372549018863</v>
+        <v>0.78431372549018863</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C87">
         <f t="shared" si="1"/>
-        <v>0.12970168612191224</v>
+        <v>-0.12970168612191224</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="C88">
         <f t="shared" si="1"/>
-        <v>-1.1688311688311761</v>
+        <v>1.1688311688311761</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2612,7 +2612,7 @@
       </c>
       <c r="C89">
         <f t="shared" si="1"/>
-        <v>0.51347881899872361</v>
+        <v>-0.51347881899872361</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -2624,7 +2624,7 @@
       </c>
       <c r="C90">
         <f t="shared" si="1"/>
-        <v>-0.38709677419354471</v>
+        <v>0.38709677419354471</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -2636,7 +2636,7 @@
       </c>
       <c r="C91">
         <f t="shared" si="1"/>
-        <v>0.89974293059126331</v>
+        <v>-0.89974293059126331</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -2648,7 +2648,7 @@
       </c>
       <c r="C92">
         <f t="shared" si="1"/>
-        <v>-2.3346303501945673</v>
+        <v>2.3346303501945673</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -2660,7 +2660,7 @@
       </c>
       <c r="C93">
         <f t="shared" si="1"/>
-        <v>1.7743979721166103</v>
+        <v>-1.7743979721166103</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2672,7 +2672,7 @@
       </c>
       <c r="C94">
         <f t="shared" si="1"/>
-        <v>1.0322580645161255</v>
+        <v>-1.0322580645161255</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2684,7 +2684,7 @@
       </c>
       <c r="C95">
         <f t="shared" si="1"/>
-        <v>-0.5215123859191545</v>
+        <v>0.5215123859191545</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -2696,7 +2696,7 @@
       </c>
       <c r="C96">
         <f t="shared" si="1"/>
-        <v>1.2970168612191959</v>
+        <v>-1.2970168612191959</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2708,7 +2708,7 @@
       </c>
       <c r="C97">
         <f t="shared" si="1"/>
-        <v>-0.26281208935611411</v>
+        <v>0.26281208935611411</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2720,7 +2720,7 @@
       </c>
       <c r="C98">
         <f t="shared" si="1"/>
-        <v>-1.7038007863695901</v>
+        <v>1.7038007863695901</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -2732,7 +2732,7 @@
       </c>
       <c r="C99">
         <f t="shared" si="1"/>
-        <v>1.8041237113401953</v>
+        <v>-1.8041237113401953</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -2744,7 +2744,7 @@
       </c>
       <c r="C100">
         <f t="shared" si="1"/>
-        <v>-0.65616797900262469</v>
+        <v>0.65616797900262469</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2756,7 +2756,7 @@
       </c>
       <c r="C101">
         <f t="shared" si="1"/>
-        <v>-0.91264667535854349</v>
+        <v>0.91264667535854349</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="C102">
         <f t="shared" si="1"/>
-        <v>-0.3875968992248025</v>
+        <v>0.3875968992248025</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -2780,7 +2780,7 @@
       </c>
       <c r="C103">
         <f t="shared" si="1"/>
-        <v>0.12870012870013967</v>
+        <v>-0.12870012870013967</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="C104">
         <f t="shared" si="1"/>
-        <v>-0.77319587628867081</v>
+        <v>0.77319587628867081</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="C105">
         <f t="shared" si="1"/>
-        <v>-0.89514066496164046</v>
+        <v>0.89514066496164046</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -2816,7 +2816,7 @@
       </c>
       <c r="C106">
         <f t="shared" si="1"/>
-        <v>0.50697084917617952</v>
+        <v>-0.50697084917617952</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -2828,7 +2828,7 @@
       </c>
       <c r="C107">
         <f t="shared" si="1"/>
-        <v>-1.1464968152866315</v>
+        <v>1.1464968152866315</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -2840,7 +2840,7 @@
       </c>
       <c r="C108">
         <f t="shared" si="1"/>
-        <v>-0.12594458438286438</v>
+        <v>0.12594458438286438</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -2852,7 +2852,7 @@
       </c>
       <c r="C109">
         <f t="shared" si="1"/>
-        <v>-0.12578616352200545</v>
+        <v>0.12578616352200545</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -2864,7 +2864,7 @@
       </c>
       <c r="C110">
         <f t="shared" si="1"/>
-        <v>0.75376884422109847</v>
+        <v>-0.75376884422109847</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="C111">
         <f t="shared" si="1"/>
-        <v>-2.1518987341772187</v>
+        <v>2.1518987341772187</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -2888,7 +2888,7 @@
       </c>
       <c r="C112">
         <f t="shared" si="1"/>
-        <v>0.12391573729864749</v>
+        <v>-0.12391573729864749</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -2900,7 +2900,7 @@
       </c>
       <c r="C113">
         <f t="shared" si="1"/>
-        <v>-1.4888337468982666</v>
+        <v>1.4888337468982666</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -2912,7 +2912,7 @@
       </c>
       <c r="C114">
         <f t="shared" si="1"/>
-        <v>-2.2004889975550088</v>
+        <v>2.2004889975550088</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -2924,7 +2924,7 @@
       </c>
       <c r="C115">
         <f t="shared" si="1"/>
-        <v>2.7511961722488003</v>
+        <v>-2.7511961722488003</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -2936,7 +2936,7 @@
       </c>
       <c r="C116">
         <f t="shared" si="1"/>
-        <v>-2.4600246002460024</v>
+        <v>2.4600246002460024</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="C117">
         <f t="shared" si="1"/>
-        <v>-0.60024009603841544</v>
+        <v>0.60024009603841544</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -2960,7 +2960,7 @@
       </c>
       <c r="C118">
         <f t="shared" si="1"/>
-        <v>-0.11933174224344693</v>
+        <v>0.11933174224344693</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -2972,7 +2972,7 @@
       </c>
       <c r="C119">
         <f t="shared" si="1"/>
-        <v>0.35756853396902422</v>
+        <v>-0.35756853396902422</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -2984,7 +2984,7 @@
       </c>
       <c r="C120">
         <f t="shared" si="1"/>
-        <v>-0.47846889952153793</v>
+        <v>0.47846889952153793</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="C121">
         <f t="shared" si="1"/>
-        <v>-0.47619047619048299</v>
+        <v>0.47619047619048299</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="C122">
         <f t="shared" si="1"/>
-        <v>0.35545023696683808</v>
+        <v>-0.35545023696683808</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="C123">
         <f t="shared" si="1"/>
-        <v>-1.0701545778834789</v>
+        <v>1.0701545778834789</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -3032,7 +3032,7 @@
       </c>
       <c r="C124">
         <f t="shared" si="1"/>
-        <v>1.2941176470588167</v>
+        <v>-1.2941176470588167</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -3044,7 +3044,7 @@
       </c>
       <c r="C125">
         <f t="shared" si="1"/>
-        <v>1.1918951132300357</v>
+        <v>-1.1918951132300357</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -3056,7 +3056,7 @@
       </c>
       <c r="C126">
         <f t="shared" si="1"/>
-        <v>-0.84439083232809242</v>
+        <v>0.84439083232809242</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -3080,7 +3080,7 @@
       </c>
       <c r="C128">
         <f t="shared" si="1"/>
-        <v>2.5119617224880315</v>
+        <v>-2.5119617224880315</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -3092,7 +3092,7 @@
       </c>
       <c r="C129">
         <f t="shared" si="1"/>
-        <v>-2.6993865030674882</v>
+        <v>2.6993865030674882</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="C130">
         <f t="shared" si="1"/>
-        <v>1.4336917562724047</v>
+        <v>-1.4336917562724047</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -3116,7 +3116,7 @@
       </c>
       <c r="C131">
         <f t="shared" si="1"/>
-        <v>1.8181818181818181</v>
+        <v>-1.8181818181818181</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -3127,8 +3127,8 @@
         <v>80.2</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C195" si="2">(B131-B132)/B131*100</f>
-        <v>0.98765432098765082</v>
+        <f t="shared" ref="C132:C195" si="2" xml:space="preserve"> (B132-B131)/B131*100</f>
+        <v>-0.98765432098765082</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -3140,7 +3140,7 @@
       </c>
       <c r="C133">
         <f t="shared" si="2"/>
-        <v>-0.99750623441396158</v>
+        <v>0.99750623441396158</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -3152,7 +3152,7 @@
       </c>
       <c r="C134">
         <f t="shared" si="2"/>
-        <v>0.12345679012344976</v>
+        <v>-0.12345679012344976</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -3164,7 +3164,7 @@
       </c>
       <c r="C135">
         <f t="shared" si="2"/>
-        <v>-0.12360939431396083</v>
+        <v>0.12360939431396083</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="C136">
         <f t="shared" si="2"/>
-        <v>-0.61728395061728392</v>
+        <v>0.61728395061728392</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C137">
         <f t="shared" si="2"/>
-        <v>-0.368098159509199</v>
+        <v>0.368098159509199</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -3200,7 +3200,7 @@
       </c>
       <c r="C138">
         <f t="shared" si="2"/>
-        <v>0.85574572127139703</v>
+        <v>-0.85574572127139703</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -3212,7 +3212,7 @@
       </c>
       <c r="C139">
         <f t="shared" si="2"/>
-        <v>-1.972872996300874</v>
+        <v>1.972872996300874</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -3224,7 +3224,7 @@
       </c>
       <c r="C140">
         <f t="shared" si="2"/>
-        <v>1.4510278113663879</v>
+        <v>-1.4510278113663879</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="C141">
         <f t="shared" si="2"/>
-        <v>-2.0858895705521507</v>
+        <v>2.0858895705521507</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="C142">
         <f t="shared" si="2"/>
-        <v>0.96153846153845812</v>
+        <v>-0.96153846153845812</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="C143">
         <f t="shared" si="2"/>
-        <v>0.84951456310679951</v>
+        <v>-0.84951456310679951</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -3272,7 +3272,7 @@
       </c>
       <c r="C144">
         <f t="shared" si="2"/>
-        <v>-1.4687882496940059</v>
+        <v>1.4687882496940059</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
@@ -3284,7 +3284,7 @@
       </c>
       <c r="C145">
         <f t="shared" si="2"/>
-        <v>1.6887816646562188</v>
+        <v>-1.6887816646562188</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
@@ -3296,7 +3296,7 @@
       </c>
       <c r="C146">
         <f t="shared" si="2"/>
-        <v>-0.98159509202453643</v>
+        <v>0.98159509202453643</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -3308,7 +3308,7 @@
       </c>
       <c r="C147">
         <f t="shared" si="2"/>
-        <v>-0.24301336573511889</v>
+        <v>0.24301336573511889</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
@@ -3332,7 +3332,7 @@
       </c>
       <c r="C149">
         <f t="shared" si="2"/>
-        <v>0.3636363636363602</v>
+        <v>-0.3636363636363602</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
@@ -3344,7 +3344,7 @@
       </c>
       <c r="C150">
         <f t="shared" si="2"/>
-        <v>0.60827250608272498</v>
+        <v>-0.60827250608272498</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
@@ -3356,7 +3356,7 @@
       </c>
       <c r="C151">
         <f t="shared" si="2"/>
-        <v>0.61199510403916768</v>
+        <v>-0.61199510403916768</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -3368,7 +3368,7 @@
       </c>
       <c r="C152">
         <f t="shared" si="2"/>
-        <v>-1.9704433497536877</v>
+        <v>1.9704433497536877</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
@@ -3380,7 +3380,7 @@
       </c>
       <c r="C153">
         <f t="shared" si="2"/>
-        <v>2.0531400966183613</v>
+        <v>-2.0531400966183613</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
@@ -3392,7 +3392,7 @@
       </c>
       <c r="C154">
         <f t="shared" si="2"/>
-        <v>0.49321824907520528</v>
+        <v>-0.49321824907520528</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="C155">
         <f t="shared" si="2"/>
-        <v>-2.726146220570016</v>
+        <v>2.726146220570016</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -3416,7 +3416,7 @@
       </c>
       <c r="C156">
         <f t="shared" si="2"/>
-        <v>-0.72376357056694118</v>
+        <v>0.72376357056694118</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="C157">
         <f t="shared" si="2"/>
-        <v>-0.4790419161676715</v>
+        <v>0.4790419161676715</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
@@ -3440,7 +3440,7 @@
       </c>
       <c r="C158">
         <f t="shared" si="2"/>
-        <v>-0.11918951132299678</v>
+        <v>0.11918951132299678</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
@@ -3452,7 +3452,7 @@
       </c>
       <c r="C159">
         <f t="shared" si="2"/>
-        <v>-0.2380952380952415</v>
+        <v>0.2380952380952415</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
@@ -3464,7 +3464,7 @@
       </c>
       <c r="C160">
         <f t="shared" si="2"/>
-        <v>0.83135391923990831</v>
+        <v>-0.83135391923990831</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="C161">
         <f t="shared" si="2"/>
-        <v>-1.4371257485029976</v>
+        <v>1.4371257485029976</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="C162">
         <f t="shared" si="2"/>
-        <v>-0.94451003541912293</v>
+        <v>0.94451003541912293</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
@@ -3500,7 +3500,7 @@
       </c>
       <c r="C163">
         <f t="shared" si="2"/>
-        <v>0.81871345029240106</v>
+        <v>-0.81871345029240106</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
@@ -3512,7 +3512,7 @@
       </c>
       <c r="C164">
         <f t="shared" si="2"/>
-        <v>-1.2971698113207648</v>
+        <v>1.2971698113207648</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
@@ -3524,7 +3524,7 @@
       </c>
       <c r="C165">
         <f t="shared" si="2"/>
-        <v>1.0477299185099018</v>
+        <v>-1.0477299185099018</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
@@ -3536,7 +3536,7 @@
       </c>
       <c r="C166">
         <f t="shared" si="2"/>
-        <v>0.23529411764706218</v>
+        <v>-0.23529411764706218</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
@@ -3548,7 +3548,7 @@
       </c>
       <c r="C167">
         <f t="shared" si="2"/>
-        <v>-1.2971698113207648</v>
+        <v>1.2971698113207648</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
@@ -3560,7 +3560,7 @@
       </c>
       <c r="C168">
         <f t="shared" si="2"/>
-        <v>1.6298020954598436</v>
+        <v>-1.6298020954598436</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
@@ -3584,7 +3584,7 @@
       </c>
       <c r="C170">
         <f t="shared" si="2"/>
-        <v>-2.2485207100591782</v>
+        <v>2.2485207100591782</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
@@ -3596,7 +3596,7 @@
       </c>
       <c r="C171">
         <f t="shared" si="2"/>
-        <v>1.0416666666666732</v>
+        <v>-1.0416666666666732</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
@@ -3608,7 +3608,7 @@
       </c>
       <c r="C172">
         <f t="shared" si="2"/>
-        <v>-0.93567251461987977</v>
+        <v>0.93567251461987977</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
@@ -3620,7 +3620,7 @@
       </c>
       <c r="C173">
         <f t="shared" si="2"/>
-        <v>-0.81112398609502057</v>
+        <v>0.81112398609502057</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
@@ -3632,7 +3632,7 @@
       </c>
       <c r="C174">
         <f t="shared" si="2"/>
-        <v>1.1494252873563218</v>
+        <v>-1.1494252873563218</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
@@ -3644,7 +3644,7 @@
       </c>
       <c r="C175">
         <f t="shared" si="2"/>
-        <v>-1.9767441860465151</v>
+        <v>1.9767441860465151</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
@@ -3656,7 +3656,7 @@
       </c>
       <c r="C176">
         <f t="shared" si="2"/>
-        <v>-1.3683010262257729</v>
+        <v>1.3683010262257729</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
@@ -3668,7 +3668,7 @@
       </c>
       <c r="C177">
         <f t="shared" si="2"/>
-        <v>2.6996625421822333</v>
+        <v>-2.6996625421822333</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
@@ -3680,7 +3680,7 @@
       </c>
       <c r="C178">
         <f t="shared" si="2"/>
-        <v>-2.4277456647398781</v>
+        <v>2.4277456647398781</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
@@ -3692,7 +3692,7 @@
       </c>
       <c r="C179">
         <f t="shared" si="2"/>
-        <v>-1.8058690744921093</v>
+        <v>1.8058690744921093</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="C180">
         <f t="shared" si="2"/>
-        <v>0.88691796008868873</v>
+        <v>-0.88691796008868873</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
@@ -3728,7 +3728,7 @@
       </c>
       <c r="C182">
         <f t="shared" si="2"/>
-        <v>-1.0067114093959635</v>
+        <v>1.0067114093959635</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
@@ -3740,7 +3740,7 @@
       </c>
       <c r="C183">
         <f t="shared" si="2"/>
-        <v>-0.22148394241417813</v>
+        <v>0.22148394241417813</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
@@ -3752,7 +3752,7 @@
       </c>
       <c r="C184">
         <f t="shared" si="2"/>
-        <v>0.88397790055248315</v>
+        <v>-0.88397790055248315</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
@@ -3764,7 +3764,7 @@
       </c>
       <c r="C185">
         <f t="shared" si="2"/>
-        <v>-2.0066889632106992</v>
+        <v>2.0066889632106992</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
@@ -3776,7 +3776,7 @@
       </c>
       <c r="C186">
         <f t="shared" si="2"/>
-        <v>-0.98360655737705538</v>
+        <v>0.98360655737705538</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C187">
         <f t="shared" si="2"/>
-        <v>0.324675324675337</v>
+        <v>-0.324675324675337</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
@@ -3800,7 +3800,7 @@
       </c>
       <c r="C188">
         <f t="shared" si="2"/>
-        <v>-1.6286644951140066</v>
+        <v>1.6286644951140066</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
@@ -3812,7 +3812,7 @@
       </c>
       <c r="C189">
         <f t="shared" si="2"/>
-        <v>-0.53418803418803418</v>
+        <v>0.53418803418803418</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
@@ -3824,7 +3824,7 @@
       </c>
       <c r="C190">
         <f t="shared" si="2"/>
-        <v>0.3188097768331532</v>
+        <v>-0.3188097768331532</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
@@ -3836,7 +3836,7 @@
       </c>
       <c r="C191">
         <f t="shared" si="2"/>
-        <v>0.42643923240937254</v>
+        <v>-0.42643923240937254</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C192">
         <f t="shared" si="2"/>
-        <v>-1.8201284796573753</v>
+        <v>1.8201284796573753</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
@@ -3860,7 +3860,7 @@
       </c>
       <c r="C193">
         <f t="shared" si="2"/>
-        <v>-0.8412197686645756</v>
+        <v>0.8412197686645756</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C194">
         <f t="shared" si="2"/>
-        <v>0.20855057351408013</v>
+        <v>-0.20855057351408013</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
@@ -3884,7 +3884,7 @@
       </c>
       <c r="C195">
         <f t="shared" si="2"/>
-        <v>-0.83594566353186739</v>
+        <v>0.83594566353186739</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
@@ -3895,8 +3895,8 @@
         <v>97</v>
       </c>
       <c r="C196">
-        <f t="shared" ref="C196:C259" si="3">(B195-B196)/B195*100</f>
-        <v>-0.5181347150259068</v>
+        <f t="shared" ref="C196:C259" si="3" xml:space="preserve"> (B196-B195)/B195*100</f>
+        <v>0.5181347150259068</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
@@ -3908,7 +3908,7 @@
       </c>
       <c r="C197">
         <f t="shared" si="3"/>
-        <v>0.82474226804123418</v>
+        <v>-0.82474226804123418</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
@@ -3920,7 +3920,7 @@
       </c>
       <c r="C198">
         <f t="shared" si="3"/>
-        <v>-1.8711018711018681</v>
+        <v>1.8711018711018681</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
@@ -3932,7 +3932,7 @@
       </c>
       <c r="C199">
         <f t="shared" si="3"/>
-        <v>-0.20408163265306412</v>
+        <v>0.20408163265306412</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
@@ -3944,7 +3944,7 @@
       </c>
       <c r="C200">
         <f t="shared" si="3"/>
-        <v>-0.61099796334011636</v>
+        <v>0.61099796334011636</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
@@ -3956,7 +3956,7 @@
       </c>
       <c r="C201">
         <f t="shared" si="3"/>
-        <v>-0.2024291497975737</v>
+        <v>0.2024291497975737</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
@@ -3968,7 +3968,7 @@
       </c>
       <c r="C202">
         <f t="shared" si="3"/>
-        <v>-0.90909090909091472</v>
+        <v>0.90909090909091472</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
@@ -3980,7 +3980,7 @@
       </c>
       <c r="C203">
         <f t="shared" si="3"/>
-        <v>-0.2002002002001888</v>
+        <v>0.2002002002001888</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
@@ -3992,7 +3992,7 @@
       </c>
       <c r="C204">
         <f t="shared" si="3"/>
-        <v>0.29970029970029688</v>
+        <v>-0.29970029970029688</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
@@ -4004,7 +4004,7 @@
       </c>
       <c r="C205">
         <f t="shared" si="3"/>
-        <v>-0.80160320641282279</v>
+        <v>0.80160320641282279</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
@@ -4016,7 +4016,7 @@
       </c>
       <c r="C206">
         <f t="shared" si="3"/>
-        <v>-0.99403578528827041</v>
+        <v>0.99403578528827041</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="C207">
         <f t="shared" si="3"/>
-        <v>0.39370078740156644</v>
+        <v>-0.39370078740156644</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
@@ -4040,7 +4040,7 @@
       </c>
       <c r="C208">
         <f t="shared" si="3"/>
-        <v>0.19762845849802652</v>
+        <v>-0.19762845849802652</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
@@ -4052,7 +4052,7 @@
       </c>
       <c r="C209">
         <f t="shared" si="3"/>
-        <v>-0.59405940594058848</v>
+        <v>0.59405940594058848</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
@@ -4064,7 +4064,7 @@
       </c>
       <c r="C210">
         <f t="shared" si="3"/>
-        <v>2.2637795275590524</v>
+        <v>-2.2637795275590524</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
@@ -4076,7 +4076,7 @@
       </c>
       <c r="C211">
         <f t="shared" si="3"/>
-        <v>-1.0070493454179255</v>
+        <v>1.0070493454179255</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C212">
         <f t="shared" si="3"/>
-        <v>1.4955134596211366</v>
+        <v>-1.4955134596211366</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
@@ -4100,7 +4100,7 @@
       </c>
       <c r="C213">
         <f t="shared" si="3"/>
-        <v>-1.6194331983805754</v>
+        <v>1.6194331983805754</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
@@ -4112,7 +4112,7 @@
       </c>
       <c r="C214">
         <f t="shared" si="3"/>
-        <v>1.8924302788844678</v>
+        <v>-1.8924302788844678</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
@@ -4124,7 +4124,7 @@
       </c>
       <c r="C215">
         <f t="shared" si="3"/>
-        <v>2.1319796954314665</v>
+        <v>-2.1319796954314665</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
@@ -4136,7 +4136,7 @@
       </c>
       <c r="C216">
         <f t="shared" si="3"/>
-        <v>4.4605809128630813</v>
+        <v>-4.4605809128630813</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
@@ -4148,7 +4148,7 @@
       </c>
       <c r="C217">
         <f t="shared" si="3"/>
-        <v>3.5830618892508119</v>
+        <v>-3.5830618892508119</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
@@ -4160,7 +4160,7 @@
       </c>
       <c r="C218">
         <f t="shared" si="3"/>
-        <v>6.9819819819819857</v>
+        <v>-6.9819819819819857</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
@@ -4172,7 +4172,7 @@
       </c>
       <c r="C219">
         <f t="shared" si="3"/>
-        <v>3.1476997578692427</v>
+        <v>-3.1476997578692427</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
@@ -4196,7 +4196,7 @@
       </c>
       <c r="C221">
         <f t="shared" si="3"/>
-        <v>3.0000000000000071</v>
+        <v>-3.0000000000000071</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
@@ -4208,7 +4208,7 @@
       </c>
       <c r="C222">
         <f t="shared" si="3"/>
-        <v>-4.3814432989690797</v>
+        <v>4.3814432989690797</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
@@ -4220,7 +4220,7 @@
       </c>
       <c r="C223">
         <f t="shared" si="3"/>
-        <v>-1.604938271604935</v>
+        <v>1.604938271604935</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
@@ -4232,7 +4232,7 @@
       </c>
       <c r="C224">
         <f t="shared" si="3"/>
-        <v>1.0935601458080091</v>
+        <v>-1.0935601458080091</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
@@ -4244,7 +4244,7 @@
       </c>
       <c r="C225">
         <f t="shared" si="3"/>
-        <v>-1.3513513513513442</v>
+        <v>1.3513513513513442</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
@@ -4256,7 +4256,7 @@
       </c>
       <c r="C226">
         <f t="shared" si="3"/>
-        <v>-3.9999999999999964</v>
+        <v>3.9999999999999964</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
@@ -4268,7 +4268,7 @@
       </c>
       <c r="C227">
         <f t="shared" si="3"/>
-        <v>1.9813519813519846</v>
+        <v>-1.9813519813519846</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
@@ -4280,7 +4280,7 @@
       </c>
       <c r="C228">
         <f t="shared" si="3"/>
-        <v>-0.59453032104637338</v>
+        <v>0.59453032104637338</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
@@ -4292,7 +4292,7 @@
       </c>
       <c r="C229">
         <f t="shared" si="3"/>
-        <v>-0.47281323877069231</v>
+        <v>0.47281323877069231</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
@@ -4304,7 +4304,7 @@
       </c>
       <c r="C230">
         <f t="shared" si="3"/>
-        <v>-1.4117647058823564</v>
+        <v>1.4117647058823564</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
@@ -4316,7 +4316,7 @@
       </c>
       <c r="C231">
         <f t="shared" si="3"/>
-        <v>1.0440835266821411</v>
+        <v>-1.0440835266821411</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
@@ -4328,7 +4328,7 @@
       </c>
       <c r="C232">
         <f t="shared" si="3"/>
-        <v>-2.3446658851113718</v>
+        <v>2.3446658851113718</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="C233">
         <f t="shared" si="3"/>
-        <v>-2.0618556701030895</v>
+        <v>2.0618556701030895</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
@@ -4352,7 +4352,7 @@
       </c>
       <c r="C234">
         <f t="shared" si="3"/>
-        <v>-3.142536475869822</v>
+        <v>3.142536475869822</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
@@ -4364,7 +4364,7 @@
       </c>
       <c r="C235">
         <f t="shared" si="3"/>
-        <v>0.97932535364527273</v>
+        <v>-0.97932535364527273</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
@@ -4388,7 +4388,7 @@
       </c>
       <c r="C237">
         <f t="shared" si="3"/>
-        <v>-1.3186813186813218</v>
+        <v>1.3186813186813218</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
@@ -4400,7 +4400,7 @@
       </c>
       <c r="C238">
         <f t="shared" si="3"/>
-        <v>-1.1930585683297117</v>
+        <v>1.1930585683297117</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="C239">
         <f t="shared" si="3"/>
-        <v>-2.1436227224008575</v>
+        <v>2.1436227224008575</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
@@ -4424,7 +4424,7 @@
       </c>
       <c r="C240">
         <f t="shared" si="3"/>
-        <v>0.52465897166841557</v>
+        <v>-0.52465897166841557</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
@@ -4436,7 +4436,7 @@
       </c>
       <c r="C241">
         <f t="shared" si="3"/>
-        <v>-1.8987341772151869</v>
+        <v>1.8987341772151869</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
@@ -4448,7 +4448,7 @@
       </c>
       <c r="C242">
         <f t="shared" si="3"/>
-        <v>0.72463768115940863</v>
+        <v>-0.72463768115940863</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
@@ -4460,7 +4460,7 @@
       </c>
       <c r="C243">
         <f t="shared" si="3"/>
-        <v>-1.0427528675703857</v>
+        <v>1.0427528675703857</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
@@ -4472,7 +4472,7 @@
       </c>
       <c r="C244">
         <f t="shared" si="3"/>
-        <v>-0.41279669762641019</v>
+        <v>0.41279669762641019</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
@@ -4484,7 +4484,7 @@
       </c>
       <c r="C245">
         <f t="shared" si="3"/>
-        <v>-0.20554984583761854</v>
+        <v>0.20554984583761854</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
@@ -4496,7 +4496,7 @@
       </c>
       <c r="C246">
         <f t="shared" si="3"/>
-        <v>-0.9230769230769289</v>
+        <v>0.9230769230769289</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
@@ -4508,7 +4508,7 @@
       </c>
       <c r="C247">
         <f t="shared" si="3"/>
-        <v>1.524390243902439</v>
+        <v>-1.524390243902439</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
@@ -4520,7 +4520,7 @@
       </c>
       <c r="C248">
         <f t="shared" si="3"/>
-        <v>-3.1991744066047412</v>
+        <v>3.1991744066047412</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
@@ -4532,7 +4532,7 @@
       </c>
       <c r="C249">
         <f t="shared" si="3"/>
-        <v>0.79999999999999727</v>
+        <v>-0.79999999999999727</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
@@ -4544,7 +4544,7 @@
       </c>
       <c r="C250">
         <f t="shared" si="3"/>
-        <v>1.6129032258064602</v>
+        <v>-1.6129032258064602</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="C251">
         <f t="shared" si="3"/>
-        <v>-1.2295081967213144</v>
+        <v>1.2295081967213144</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
@@ -4568,7 +4568,7 @@
       </c>
       <c r="C252">
         <f t="shared" si="3"/>
-        <v>0.70850202429150089</v>
+        <v>-0.70850202429150089</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
@@ -4580,7 +4580,7 @@
       </c>
       <c r="C253">
         <f t="shared" si="3"/>
-        <v>1.1213047910295559</v>
+        <v>-1.1213047910295559</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
@@ -4592,7 +4592,7 @@
       </c>
       <c r="C254">
         <f t="shared" si="3"/>
-        <v>-0.41237113402062436</v>
+        <v>0.41237113402062436</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
@@ -4604,7 +4604,7 @@
       </c>
       <c r="C255">
         <f t="shared" si="3"/>
-        <v>-0.51334702258726894</v>
+        <v>0.51334702258726894</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
@@ -4616,7 +4616,7 @@
       </c>
       <c r="C256">
         <f t="shared" si="3"/>
-        <v>-0.71501532175688309</v>
+        <v>0.71501532175688309</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
@@ -4628,7 +4628,7 @@
       </c>
       <c r="C257">
         <f t="shared" si="3"/>
-        <v>1.4198782961460361</v>
+        <v>-1.4198782961460361</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
@@ -4640,7 +4640,7 @@
       </c>
       <c r="C258">
         <f t="shared" si="3"/>
-        <v>-1.6460905349794182</v>
+        <v>1.6460905349794182</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
@@ -4652,7 +4652,7 @@
       </c>
       <c r="C259">
         <f t="shared" si="3"/>
-        <v>1.1133603238866339</v>
+        <v>-1.1133603238866339</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
@@ -4663,8 +4663,8 @@
         <v>98.5</v>
       </c>
       <c r="C260">
-        <f t="shared" ref="C260:C323" si="4">(B259-B260)/B259*100</f>
-        <v>-0.81883316274308815</v>
+        <f t="shared" ref="C260:C323" si="4" xml:space="preserve"> (B260-B259)/B259*100</f>
+        <v>0.81883316274308815</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
@@ -4676,7 +4676,7 @@
       </c>
       <c r="C261">
         <f t="shared" si="4"/>
-        <v>-0.2030456852791907</v>
+        <v>0.2030456852791907</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
@@ -4688,7 +4688,7 @@
       </c>
       <c r="C262">
         <f t="shared" si="4"/>
-        <v>1.2158054711246229</v>
+        <v>-1.2158054711246229</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
@@ -4700,7 +4700,7 @@
       </c>
       <c r="C263">
         <f t="shared" si="4"/>
-        <v>1.4358974358974419</v>
+        <v>-1.4358974358974419</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
@@ -4712,7 +4712,7 @@
       </c>
       <c r="C264">
         <f t="shared" si="4"/>
-        <v>0.62434963579603997</v>
+        <v>-0.62434963579603997</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
@@ -4724,7 +4724,7 @@
       </c>
       <c r="C265">
         <f t="shared" si="4"/>
-        <v>-0.41884816753927295</v>
+        <v>0.41884816753927295</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
@@ -4736,7 +4736,7 @@
       </c>
       <c r="C266">
         <f t="shared" si="4"/>
-        <v>0.83420229405632051</v>
+        <v>-0.83420229405632051</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="C267">
         <f t="shared" si="4"/>
-        <v>-0.73606729758149625</v>
+        <v>0.73606729758149625</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
@@ -4760,7 +4760,7 @@
       </c>
       <c r="C268">
         <f t="shared" si="4"/>
-        <v>-1.7745302713987505</v>
+        <v>1.7745302713987505</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
@@ -4772,7 +4772,7 @@
       </c>
       <c r="C269">
         <f t="shared" si="4"/>
-        <v>0.10256410256409673</v>
+        <v>-0.10256410256409673</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
@@ -4784,7 +4784,7 @@
       </c>
       <c r="C270">
         <f t="shared" si="4"/>
-        <v>0.82135523613964201</v>
+        <v>-0.82135523613964201</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
@@ -4796,7 +4796,7 @@
       </c>
       <c r="C271">
         <f t="shared" si="4"/>
-        <v>-1.759834368530024</v>
+        <v>1.759834368530024</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
@@ -4808,7 +4808,7 @@
       </c>
       <c r="C272">
         <f t="shared" si="4"/>
-        <v>1.5259409969481181</v>
+        <v>-1.5259409969481181</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
@@ -4820,7 +4820,7 @@
       </c>
       <c r="C273">
         <f t="shared" si="4"/>
-        <v>-1.9628099173553779</v>
+        <v>1.9628099173553779</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
@@ -4832,7 +4832,7 @@
       </c>
       <c r="C274">
         <f t="shared" si="4"/>
-        <v>0.30395136778115212</v>
+        <v>-0.30395136778115212</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
@@ -4844,7 +4844,7 @@
       </c>
       <c r="C275">
         <f t="shared" si="4"/>
-        <v>0.71138211382114103</v>
+        <v>-0.71138211382114103</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
@@ -4856,7 +4856,7 @@
       </c>
       <c r="C276">
         <f t="shared" si="4"/>
-        <v>-1.7400204708290714</v>
+        <v>1.7400204708290714</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
@@ -4868,7 +4868,7 @@
       </c>
       <c r="C277">
         <f t="shared" si="4"/>
-        <v>-0.20120724346075317</v>
+        <v>0.20120724346075317</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
@@ -4880,7 +4880,7 @@
       </c>
       <c r="C278">
         <f t="shared" si="4"/>
-        <v>0.70281124497990832</v>
+        <v>-0.70281124497990832</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
@@ -4904,7 +4904,7 @@
       </c>
       <c r="C280">
         <f t="shared" si="4"/>
-        <v>-0.30333670374114979</v>
+        <v>0.30333670374114979</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
@@ -4916,7 +4916,7 @@
       </c>
       <c r="C281">
         <f t="shared" si="4"/>
-        <v>0.4032258064516186</v>
+        <v>-0.4032258064516186</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
@@ -4928,7 +4928,7 @@
       </c>
       <c r="C282">
         <f t="shared" si="4"/>
-        <v>0.50607287449392713</v>
+        <v>-0.50607287449392713</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
@@ -4940,7 +4940,7 @@
       </c>
       <c r="C283">
         <f t="shared" si="4"/>
-        <v>-0.10172939979654987</v>
+        <v>0.10172939979654987</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
@@ -4952,7 +4952,7 @@
       </c>
       <c r="C284">
         <f t="shared" si="4"/>
-        <v>-1.6260162601625958</v>
+        <v>1.6260162601625958</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
@@ -4964,7 +4964,7 @@
       </c>
       <c r="C285">
         <f t="shared" si="4"/>
-        <v>3.5000000000000004</v>
+        <v>-3.5000000000000004</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
@@ -4976,7 +4976,7 @@
       </c>
       <c r="C286">
         <f t="shared" si="4"/>
-        <v>-2.4870466321243581</v>
+        <v>2.4870466321243581</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="C287">
         <f t="shared" si="4"/>
-        <v>-0.30333670374114979</v>
+        <v>0.30333670374114979</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
@@ -5000,7 +5000,7 @@
       </c>
       <c r="C288">
         <f t="shared" si="4"/>
-        <v>0.10080645161291181</v>
+        <v>-0.10080645161291181</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
@@ -5012,7 +5012,7 @@
       </c>
       <c r="C289">
         <f t="shared" si="4"/>
-        <v>-1.7154389505549978</v>
+        <v>1.7154389505549978</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
@@ -5024,7 +5024,7 @@
       </c>
       <c r="C290">
         <f t="shared" si="4"/>
-        <v>2.3809523809523725</v>
+        <v>-2.3809523809523725</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
@@ -5036,7 +5036,7 @@
       </c>
       <c r="C291">
         <f t="shared" si="4"/>
-        <v>-1.0162601626016259</v>
+        <v>1.0162601626016259</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
@@ -5060,7 +5060,7 @@
       </c>
       <c r="C293">
         <f t="shared" si="4"/>
-        <v>-0.80482897384305552</v>
+        <v>0.80482897384305552</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
@@ -5072,7 +5072,7 @@
       </c>
       <c r="C294">
         <f t="shared" si="4"/>
-        <v>-9.9800399201591145E-2</v>
+        <v>9.9800399201591145E-2</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
@@ -5096,7 +5096,7 @@
       </c>
       <c r="C296">
         <f t="shared" si="4"/>
-        <v>-1.3958125623130666</v>
+        <v>1.3958125623130666</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
@@ -5108,7 +5108,7 @@
       </c>
       <c r="C297">
         <f t="shared" si="4"/>
-        <v>2.5565388397246886</v>
+        <v>-2.5565388397246886</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
@@ -5120,7 +5120,7 @@
       </c>
       <c r="C298">
         <f t="shared" si="4"/>
-        <v>-0.30272452068618705</v>
+        <v>0.30272452068618705</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
@@ -5132,7 +5132,7 @@
       </c>
       <c r="C299">
         <f t="shared" si="4"/>
-        <v>-0.80482897384305552</v>
+        <v>0.80482897384305552</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
@@ -5144,7 +5144,7 @@
       </c>
       <c r="C300">
         <f t="shared" si="4"/>
-        <v>1.1976047904191645</v>
+        <v>-1.1976047904191645</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
@@ -5156,7 +5156,7 @@
       </c>
       <c r="C301">
         <f t="shared" si="4"/>
-        <v>-0.70707070707070996</v>
+        <v>0.70707070707070996</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
@@ -5168,7 +5168,7 @@
       </c>
       <c r="C302">
         <f t="shared" si="4"/>
-        <v>-1.303911735205614</v>
+        <v>1.303911735205614</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
@@ -5180,7 +5180,7 @@
       </c>
       <c r="C303">
         <f t="shared" si="4"/>
-        <v>9.900990099009338E-2</v>
+        <v>-9.900990099009338E-2</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
@@ -5192,7 +5192,7 @@
       </c>
       <c r="C304">
         <f t="shared" si="4"/>
-        <v>0.89197224975223544</v>
+        <v>-0.89197224975223544</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
@@ -5204,7 +5204,7 @@
       </c>
       <c r="C305">
         <f t="shared" si="4"/>
-        <v>-0.70000000000000284</v>
+        <v>0.70000000000000284</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="C306">
         <f t="shared" si="4"/>
-        <v>1.6881827209533296</v>
+        <v>-1.6881827209533296</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
@@ -5228,7 +5228,7 @@
       </c>
       <c r="C307">
         <f t="shared" si="4"/>
-        <v>-2.0202020202020203</v>
+        <v>2.0202020202020203</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
@@ -5240,7 +5240,7 @@
       </c>
       <c r="C308">
         <f t="shared" si="4"/>
-        <v>1.3861386138613918</v>
+        <v>-1.3861386138613918</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
@@ -5252,7 +5252,7 @@
       </c>
       <c r="C309">
         <f t="shared" si="4"/>
-        <v>-1.6064257028112534</v>
+        <v>1.6064257028112534</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
@@ -5264,7 +5264,7 @@
       </c>
       <c r="C310">
         <f t="shared" si="4"/>
-        <v>0.19762845849802652</v>
+        <v>-0.19762845849802652</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
@@ -5276,7 +5276,7 @@
       </c>
       <c r="C311">
         <f t="shared" si="4"/>
-        <v>-0.49504950495049505</v>
+        <v>0.49504950495049505</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C312">
         <f t="shared" si="4"/>
-        <v>0.19704433497537227</v>
+        <v>-0.19704433497537227</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
@@ -5300,7 +5300,7 @@
       </c>
       <c r="C313">
         <f t="shared" si="4"/>
-        <v>1.8756169792694881</v>
+        <v>-1.8756169792694881</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
@@ -5312,7 +5312,7 @@
       </c>
       <c r="C314">
         <f t="shared" si="4"/>
-        <v>-1.4084507042253436</v>
+        <v>1.4084507042253436</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
@@ -5324,7 +5324,7 @@
       </c>
       <c r="C315">
         <f t="shared" si="4"/>
-        <v>-0.89285714285714857</v>
+        <v>0.89285714285714857</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
@@ -5336,7 +5336,7 @@
       </c>
       <c r="C316">
         <f t="shared" si="4"/>
-        <v>0.58997050147493468</v>
+        <v>-0.58997050147493468</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
@@ -5348,7 +5348,7 @@
       </c>
       <c r="C317">
         <f t="shared" si="4"/>
-        <v>-1.7804154302670738</v>
+        <v>1.7804154302670738</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
@@ -5360,7 +5360,7 @@
       </c>
       <c r="C318">
         <f t="shared" si="4"/>
-        <v>-0.38872691933915593</v>
+        <v>0.38872691933915593</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
@@ -5384,7 +5384,7 @@
       </c>
       <c r="C320">
         <f t="shared" si="4"/>
-        <v>-0.38722168441433275</v>
+        <v>0.38722168441433275</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
@@ -5396,7 +5396,7 @@
       </c>
       <c r="C321">
         <f t="shared" si="4"/>
-        <v>-2.2179363548698139</v>
+        <v>2.2179363548698139</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
@@ -5408,7 +5408,7 @@
       </c>
       <c r="C322">
         <f t="shared" si="4"/>
-        <v>1.0377358490565984</v>
+        <v>-1.0377358490565984</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
@@ -5420,7 +5420,7 @@
       </c>
       <c r="C323">
         <f t="shared" si="4"/>
-        <v>1.3346043851286995</v>
+        <v>-1.3346043851286995</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
@@ -5431,8 +5431,8 @@
         <v>107</v>
       </c>
       <c r="C324">
-        <f t="shared" ref="C324:C387" si="5">(B323-B324)/B323*100</f>
-        <v>-3.3816425120772946</v>
+        <f t="shared" ref="C324:C387" si="5" xml:space="preserve"> (B324-B323)/B323*100</f>
+        <v>3.3816425120772946</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
@@ -5444,7 +5444,7 @@
       </c>
       <c r="C325">
         <f t="shared" si="5"/>
-        <v>0.46728971962616817</v>
+        <v>-0.46728971962616817</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="C326">
         <f t="shared" si="5"/>
-        <v>0.75117370892018509</v>
+        <v>-0.75117370892018509</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
@@ -5468,7 +5468,7 @@
       </c>
       <c r="C327">
         <f t="shared" si="5"/>
-        <v>1.4191106906338693</v>
+        <v>-1.4191106906338693</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
@@ -5480,7 +5480,7 @@
       </c>
       <c r="C328">
         <f t="shared" si="5"/>
-        <v>-1.2476007677543157</v>
+        <v>1.2476007677543157</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
@@ -5492,7 +5492,7 @@
       </c>
       <c r="C329">
         <f t="shared" si="5"/>
-        <v>0.75829383886255652</v>
+        <v>-0.75829383886255652</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
@@ -5504,7 +5504,7 @@
       </c>
       <c r="C330">
         <f t="shared" si="5"/>
-        <v>-1.6236867239732597</v>
+        <v>1.6236867239732597</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
@@ -5528,7 +5528,7 @@
       </c>
       <c r="C332">
         <f t="shared" si="5"/>
-        <v>1.8796992481203008</v>
+        <v>-1.8796992481203008</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
@@ -5540,7 +5540,7 @@
       </c>
       <c r="C333">
         <f t="shared" si="5"/>
-        <v>-1.0536398467432895</v>
+        <v>1.0536398467432895</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
@@ -5552,7 +5552,7 @@
       </c>
       <c r="C334">
         <f t="shared" si="5"/>
-        <v>1.0426540284360135</v>
+        <v>-1.0426540284360135</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
@@ -5564,7 +5564,7 @@
       </c>
       <c r="C335">
         <f t="shared" si="5"/>
-        <v>0.19157088122605637</v>
+        <v>-0.19157088122605637</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
@@ -5576,7 +5576,7 @@
       </c>
       <c r="C336">
         <f t="shared" si="5"/>
-        <v>1.8234165067178558</v>
+        <v>-1.8234165067178558</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
@@ -5588,7 +5588,7 @@
       </c>
       <c r="C337">
         <f t="shared" si="5"/>
-        <v>-0.97751710654936463</v>
+        <v>0.97751710654936463</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
@@ -5600,7 +5600,7 @@
       </c>
       <c r="C338">
         <f t="shared" si="5"/>
-        <v>9.6805421103576289E-2</v>
+        <v>-9.6805421103576289E-2</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.2">
@@ -5612,7 +5612,7 @@
       </c>
       <c r="C339">
         <f t="shared" si="5"/>
-        <v>0.29069767441860189</v>
+        <v>-0.29069767441860189</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.2">
@@ -5624,7 +5624,7 @@
       </c>
       <c r="C340">
         <f t="shared" si="5"/>
-        <v>-0.68027210884352629</v>
+        <v>0.68027210884352629</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
@@ -5636,7 +5636,7 @@
       </c>
       <c r="C341">
         <f t="shared" si="5"/>
-        <v>1.6409266409266301</v>
+        <v>-1.6409266409266301</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
@@ -5648,7 +5648,7 @@
       </c>
       <c r="C342">
         <f t="shared" si="5"/>
-        <v>-0.58881256133463622</v>
+        <v>0.58881256133463622</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.2">
@@ -5660,7 +5660,7 @@
       </c>
       <c r="C343">
         <f t="shared" si="5"/>
-        <v>1.0731707317073116</v>
+        <v>-1.0731707317073116</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.2">
@@ -5672,7 +5672,7 @@
       </c>
       <c r="C344">
         <f t="shared" si="5"/>
-        <v>0.49309664694280081</v>
+        <v>-0.49309664694280081</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.2">
@@ -5684,7 +5684,7 @@
       </c>
       <c r="C345">
         <f t="shared" si="5"/>
-        <v>-0.19821605550048427</v>
+        <v>0.19821605550048427</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.2">
@@ -5696,7 +5696,7 @@
       </c>
       <c r="C346">
         <f t="shared" si="5"/>
-        <v>0.79129574678535819</v>
+        <v>-0.79129574678535819</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.2">
@@ -5708,7 +5708,7 @@
       </c>
       <c r="C347">
         <f t="shared" si="5"/>
-        <v>0.49850448654037888</v>
+        <v>-0.49850448654037888</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.2">
@@ -5720,7 +5720,7 @@
       </c>
       <c r="C348">
         <f t="shared" si="5"/>
-        <v>-0.20040080160320925</v>
+        <v>0.20040080160320925</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.2">
@@ -5732,7 +5732,7 @@
       </c>
       <c r="C349">
         <f t="shared" si="5"/>
-        <v>2.2000000000000028</v>
+        <v>-2.2000000000000028</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.2">
@@ -5744,7 +5744,7 @@
       </c>
       <c r="C350">
         <f t="shared" si="5"/>
-        <v>-2.862985685071572</v>
+        <v>2.862985685071572</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
@@ -5756,7 +5756,7 @@
       </c>
       <c r="C351">
         <f t="shared" si="5"/>
-        <v>-1.1928429423459275</v>
+        <v>1.1928429423459275</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
@@ -5768,7 +5768,7 @@
       </c>
       <c r="C352">
         <f t="shared" si="5"/>
-        <v>10.609037328094301</v>
+        <v>-10.609037328094301</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
@@ -5780,7 +5780,7 @@
       </c>
       <c r="C353">
         <f t="shared" si="5"/>
-        <v>21.538461538461533</v>
+        <v>-21.538461538461533</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
@@ -5792,7 +5792,7 @@
       </c>
       <c r="C354">
         <f t="shared" si="5"/>
-        <v>-11.484593837534996</v>
+        <v>11.484593837534996</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
@@ -5804,7 +5804,7 @@
       </c>
       <c r="C355">
         <f t="shared" si="5"/>
-        <v>-11.809045226130662</v>
+        <v>11.809045226130662</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.2">
@@ -5816,7 +5816,7 @@
       </c>
       <c r="C356">
         <f t="shared" si="5"/>
-        <v>-2.0224719101123565</v>
+        <v>2.0224719101123565</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.2">
@@ -5828,7 +5828,7 @@
       </c>
       <c r="C357">
         <f t="shared" si="5"/>
-        <v>0.44052863436122408</v>
+        <v>-0.44052863436122408</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.2">
@@ -5840,7 +5840,7 @@
       </c>
       <c r="C358">
         <f t="shared" si="5"/>
-        <v>-2.8761061946902586</v>
+        <v>2.8761061946902586</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.2">
@@ -5852,7 +5852,7 @@
       </c>
       <c r="C359">
         <f t="shared" si="5"/>
-        <v>-3.763440860215054</v>
+        <v>3.763440860215054</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
@@ -5864,7 +5864,7 @@
       </c>
       <c r="C360">
         <f t="shared" si="5"/>
-        <v>-1.243523316062179</v>
+        <v>1.243523316062179</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.2">
@@ -5888,7 +5888,7 @@
       </c>
       <c r="C362">
         <f t="shared" si="5"/>
-        <v>0.30706243602865624</v>
+        <v>-0.30706243602865624</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.2">
@@ -5900,7 +5900,7 @@
       </c>
       <c r="C363">
         <f t="shared" si="5"/>
-        <v>1.4373716632443589</v>
+        <v>-1.4373716632443589</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.2">
@@ -5912,7 +5912,7 @@
       </c>
       <c r="C364">
         <f t="shared" si="5"/>
-        <v>-1.6666666666666607</v>
+        <v>1.6666666666666607</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.2">
@@ -5924,7 +5924,7 @@
       </c>
       <c r="C365">
         <f t="shared" si="5"/>
-        <v>0.20491803278687359</v>
+        <v>-0.20491803278687359</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.2">
@@ -5936,7 +5936,7 @@
       </c>
       <c r="C366">
         <f t="shared" si="5"/>
-        <v>1.1293634496920006</v>
+        <v>-1.1293634496920006</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.2">
@@ -5948,7 +5948,7 @@
       </c>
       <c r="C367">
         <f t="shared" si="5"/>
-        <v>0.8307372793354072</v>
+        <v>-0.8307372793354072</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.2">
@@ -5960,7 +5960,7 @@
       </c>
       <c r="C368">
         <f t="shared" si="5"/>
-        <v>-1.0471204188481675</v>
+        <v>1.0471204188481675</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.2">
@@ -5972,7 +5972,7 @@
       </c>
       <c r="C369">
         <f t="shared" si="5"/>
-        <v>4.248704663212429</v>
+        <v>-4.248704663212429</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.2">
@@ -5996,7 +5996,7 @@
       </c>
       <c r="C371">
         <f t="shared" si="5"/>
-        <v>-3.1385281385281294</v>
+        <v>3.1385281385281294</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
@@ -6008,7 +6008,7 @@
       </c>
       <c r="C372">
         <f t="shared" si="5"/>
-        <v>-0.73452256033578478</v>
+        <v>0.73452256033578478</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
@@ -6020,7 +6020,7 @@
       </c>
       <c r="C373">
         <f t="shared" si="5"/>
-        <v>-1.1458333333333273</v>
+        <v>1.1458333333333273</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.2">
@@ -6032,7 +6032,7 @@
       </c>
       <c r="C374">
         <f t="shared" si="5"/>
-        <v>-0.20597322348095043</v>
+        <v>0.20597322348095043</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
@@ -6044,7 +6044,7 @@
       </c>
       <c r="C375">
         <f t="shared" si="5"/>
-        <v>-0.41109969167523708</v>
+        <v>0.41109969167523708</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
@@ -6056,7 +6056,7 @@
       </c>
       <c r="C376">
         <f t="shared" si="5"/>
-        <v>4.8106448311156633</v>
+        <v>-4.8106448311156633</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
@@ -6068,7 +6068,7 @@
       </c>
       <c r="C377">
         <f t="shared" si="5"/>
-        <v>-1.8279569892473151</v>
+        <v>1.8279569892473151</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
@@ -6080,7 +6080,7 @@
       </c>
       <c r="C378">
         <f t="shared" si="5"/>
-        <v>-0.10559662090812492</v>
+        <v>0.10559662090812492</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.2">
@@ -6092,7 +6092,7 @@
       </c>
       <c r="C379">
         <f t="shared" si="5"/>
-        <v>-1.2658227848101298</v>
+        <v>1.2658227848101298</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
@@ -6104,7 +6104,7 @@
       </c>
       <c r="C380">
         <f t="shared" si="5"/>
-        <v>0.624999999999994</v>
+        <v>-0.624999999999994</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
@@ -6116,7 +6116,7 @@
       </c>
       <c r="C381">
         <f t="shared" si="5"/>
-        <v>0.73375262054507628</v>
+        <v>-0.73375262054507628</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.2">
@@ -6128,7 +6128,7 @@
       </c>
       <c r="C382">
         <f t="shared" si="5"/>
-        <v>-1.2671594508975743</v>
+        <v>1.2671594508975743</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.2">
@@ -6140,7 +6140,7 @@
       </c>
       <c r="C383">
         <f t="shared" si="5"/>
-        <v>0.93847758081335297</v>
+        <v>-0.93847758081335297</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
@@ -6152,7 +6152,7 @@
       </c>
       <c r="C384">
         <f t="shared" si="5"/>
-        <v>-0.8421052631578918</v>
+        <v>0.8421052631578918</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.2">
@@ -6164,7 +6164,7 @@
       </c>
       <c r="C385">
         <f t="shared" si="5"/>
-        <v>1.4613778705636653</v>
+        <v>-1.4613778705636653</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.2">
@@ -6176,7 +6176,7 @@
       </c>
       <c r="C386">
         <f t="shared" si="5"/>
-        <v>-1.9067796610169461</v>
+        <v>1.9067796610169461</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.2">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C387">
         <f t="shared" si="5"/>
-        <v>-2.4948024948024861</v>
+        <v>2.4948024948024861</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.2">
@@ -6199,8 +6199,8 @@
         <v>95.5</v>
       </c>
       <c r="C388">
-        <f t="shared" ref="C388" si="6">(B387-B388)/B387*100</f>
-        <v>3.1440162271805216</v>
+        <f t="shared" ref="C388" si="6" xml:space="preserve"> (B388-B387)/B387*100</f>
+        <v>-3.1440162271805216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>